<commit_message>
added path to turn off a light control scheduler
</commit_message>
<xml_diff>
--- a/MixerTableExcels/MixerTableV2.xlsx
+++ b/MixerTableExcels/MixerTableV2.xlsx
@@ -294,10 +294,10 @@
   <dimension ref="A1:R86"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.35546875" defaultRowHeight="21.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="16.36328125" defaultRowHeight="21.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="16.36"/>
   </cols>
@@ -354,28 +354,28 @@
         <v>9</v>
       </c>
       <c r="K2" s="5" t="n">
-        <v>80</v>
+        <v>1000</v>
       </c>
       <c r="L2" s="5" t="n">
-        <v>80</v>
+        <v>1000</v>
       </c>
       <c r="M2" s="5" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="N2" s="5" t="n">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="O2" s="5" t="n">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="P2" s="5" t="n">
-        <v>80</v>
+        <v>1000</v>
       </c>
       <c r="Q2" s="5" t="n">
-        <v>30</v>
+        <v>1000</v>
       </c>
       <c r="R2" s="5" t="n">
-        <v>80</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="22.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -408,7 +408,7 @@
         <v>10</v>
       </c>
       <c r="K3" s="6" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
@@ -449,35 +449,35 @@
       </c>
       <c r="K4" s="7" t="n">
         <f aca="false">((100/MAX($K2:$R2)*K2)*10)*($K3/100)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="L4" s="7" t="n">
         <f aca="false">((100/MAX($K2:$R2)*L2)*10)*($K3/100)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="M4" s="7" t="n">
         <f aca="false">((100/MAX($K2:$R2)*M2)*10)*($K3/100)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="N4" s="7" t="n">
         <f aca="false">((100/MAX($K2:$R2)*N2)*10)*($K3/100)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="O4" s="7" t="n">
         <f aca="false">((100/MAX($K2:$R2)*O2)*10)*($K3/100)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="P4" s="7" t="n">
         <f aca="false">((100/MAX($K2:$R2)*P2)*10)*($K3/100)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="Q4" s="7" t="n">
         <f aca="false">((100/MAX($K2:$R2)*Q2)*10)*($K3/100)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="R4" s="7" t="n">
         <f aca="false">((100/MAX($K2:$R2)*R2)*10)*($K3/100)</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="50.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -519,7 +519,7 @@
       </c>
       <c r="K5" s="9" t="n">
         <f aca="false">SUM(J11:J70)</f>
-        <v>0</v>
+        <v>679.637172275645</v>
       </c>
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
@@ -557,7 +557,7 @@
       <c r="I6" s="9"/>
       <c r="J6" s="10" t="n">
         <f aca="false">A6*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B6*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C6*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D6*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E6*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F6*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G6*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H6*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>0.198718656045236</v>
       </c>
       <c r="K6" s="10"/>
       <c r="L6" s="10"/>
@@ -596,7 +596,7 @@
       <c r="I7" s="9"/>
       <c r="J7" s="9" t="n">
         <f aca="false">A7*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B7*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C7*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D7*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E7*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F7*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G7*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H7*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>0.26215594997516</v>
       </c>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
@@ -635,7 +635,7 @@
       <c r="I8" s="9"/>
       <c r="J8" s="10" t="n">
         <f aca="false">A8*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B8*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C8*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D8*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E8*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F8*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G8*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H8*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>0.592803541775983</v>
       </c>
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
@@ -674,7 +674,7 @@
       <c r="I9" s="9"/>
       <c r="J9" s="9" t="n">
         <f aca="false">A9*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B9*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C9*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D9*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E9*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F9*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G9*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H9*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>1.57071788784858</v>
       </c>
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
@@ -713,7 +713,7 @@
       <c r="I10" s="9"/>
       <c r="J10" s="10" t="n">
         <f aca="false">A10*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B10*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C10*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D10*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E10*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F10*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G10*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H10*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>4.38264068610225</v>
       </c>
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
@@ -752,7 +752,7 @@
       <c r="I11" s="9"/>
       <c r="J11" s="9" t="n">
         <f aca="false">A11*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B11*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C11*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D11*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E11*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F11*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G11*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H11*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>8.08939045209431</v>
       </c>
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
@@ -791,7 +791,7 @@
       <c r="I12" s="9"/>
       <c r="J12" s="10" t="n">
         <f aca="false">A12*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B12*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C12*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D12*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E12*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F12*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G12*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H12*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>12.7926869985735</v>
       </c>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
@@ -830,7 +830,7 @@
       <c r="I13" s="9"/>
       <c r="J13" s="9" t="n">
         <f aca="false">A13*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B13*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C13*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D13*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E13*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F13*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G13*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H13*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>14.9608124332827</v>
       </c>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
@@ -869,7 +869,7 @@
       <c r="I14" s="9"/>
       <c r="J14" s="10" t="n">
         <f aca="false">A14*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B14*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C14*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D14*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E14*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F14*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G14*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H14*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>12.927182211225</v>
       </c>
       <c r="K14" s="10"/>
       <c r="L14" s="10"/>
@@ -908,7 +908,7 @@
       <c r="I15" s="9"/>
       <c r="J15" s="9" t="n">
         <f aca="false">A15*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B15*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C15*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D15*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E15*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F15*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G15*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H15*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>9.96835627467172</v>
       </c>
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
@@ -947,7 +947,7 @@
       <c r="I16" s="9"/>
       <c r="J16" s="10" t="n">
         <f aca="false">A16*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B16*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C16*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D16*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E16*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F16*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G16*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H16*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>7.18872853236782</v>
       </c>
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
@@ -986,7 +986,7 @@
       <c r="I17" s="9"/>
       <c r="J17" s="9" t="n">
         <f aca="false">A17*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B17*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C17*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D17*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E17*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F17*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G17*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H17*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>6.03890488285416</v>
       </c>
       <c r="K17" s="9"/>
       <c r="L17" s="9"/>
@@ -1025,7 +1025,7 @@
       <c r="I18" s="9"/>
       <c r="J18" s="10" t="n">
         <f aca="false">A18*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B18*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C18*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D18*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E18*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F18*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G18*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H18*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>7.62992729726941</v>
       </c>
       <c r="K18" s="10"/>
       <c r="L18" s="10"/>
@@ -1064,7 +1064,7 @@
       <c r="I19" s="9"/>
       <c r="J19" s="9" t="n">
         <f aca="false">A19*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B19*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C19*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D19*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E19*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F19*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G19*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H19*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>9.50486145011721</v>
       </c>
       <c r="K19" s="9"/>
       <c r="L19" s="9"/>
@@ -1103,7 +1103,7 @@
       <c r="I20" s="9"/>
       <c r="J20" s="10" t="n">
         <f aca="false">A20*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B20*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C20*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D20*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E20*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F20*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G20*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H20*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>10.2625203657304</v>
       </c>
       <c r="K20" s="10"/>
       <c r="L20" s="10"/>
@@ -1142,7 +1142,7 @@
       <c r="I21" s="9"/>
       <c r="J21" s="9" t="n">
         <f aca="false">A21*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B21*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C21*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D21*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E21*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F21*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G21*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H21*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>9.54355555327564</v>
       </c>
       <c r="K21" s="9"/>
       <c r="L21" s="9"/>
@@ -1181,7 +1181,7 @@
       <c r="I22" s="9"/>
       <c r="J22" s="10" t="n">
         <f aca="false">A22*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B22*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C22*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D22*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E22*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F22*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G22*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H22*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>7.95631223600975</v>
       </c>
       <c r="K22" s="10"/>
       <c r="L22" s="10"/>
@@ -1220,7 +1220,7 @@
       <c r="I23" s="9"/>
       <c r="J23" s="9" t="n">
         <f aca="false">A23*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B23*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C23*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D23*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E23*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F23*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G23*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H23*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>6.52905714136834</v>
       </c>
       <c r="K23" s="9"/>
       <c r="L23" s="9"/>
@@ -1259,7 +1259,7 @@
       <c r="I24" s="9"/>
       <c r="J24" s="10" t="n">
         <f aca="false">A24*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B24*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C24*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D24*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E24*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F24*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G24*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H24*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>5.46767287825677</v>
       </c>
       <c r="K24" s="10"/>
       <c r="L24" s="10"/>
@@ -1298,7 +1298,7 @@
       <c r="I25" s="9"/>
       <c r="J25" s="9" t="n">
         <f aca="false">A25*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B25*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C25*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D25*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E25*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F25*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G25*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H25*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>4.74308250981637</v>
       </c>
       <c r="K25" s="9"/>
       <c r="L25" s="9"/>
@@ -1337,7 +1337,7 @@
       <c r="I26" s="9"/>
       <c r="J26" s="10" t="n">
         <f aca="false">A26*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B26*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C26*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D26*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E26*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F26*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G26*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H26*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>4.32183269371854</v>
       </c>
       <c r="K26" s="10"/>
       <c r="L26" s="10"/>
@@ -1376,7 +1376,7 @@
       <c r="I27" s="9"/>
       <c r="J27" s="9" t="n">
         <f aca="false">A27*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B27*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C27*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D27*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E27*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F27*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G27*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H27*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>4.39526561998365</v>
       </c>
       <c r="K27" s="9"/>
       <c r="L27" s="9"/>
@@ -1415,7 +1415,7 @@
       <c r="I28" s="9"/>
       <c r="J28" s="10" t="n">
         <f aca="false">A28*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B28*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C28*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D28*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E28*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F28*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G28*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H28*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>4.7985046709622</v>
       </c>
       <c r="K28" s="10"/>
       <c r="L28" s="10"/>
@@ -1454,7 +1454,7 @@
       <c r="I29" s="9"/>
       <c r="J29" s="9" t="n">
         <f aca="false">A29*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B29*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C29*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D29*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E29*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F29*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G29*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H29*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>5.30272637372881</v>
       </c>
       <c r="K29" s="9"/>
       <c r="L29" s="9"/>
@@ -1493,7 +1493,7 @@
       <c r="I30" s="9"/>
       <c r="J30" s="10" t="n">
         <f aca="false">A30*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B30*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C30*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D30*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E30*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F30*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G30*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H30*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>5.77287453757372</v>
       </c>
       <c r="K30" s="10"/>
       <c r="L30" s="10"/>
@@ -1532,7 +1532,7 @@
       <c r="I31" s="9"/>
       <c r="J31" s="9" t="n">
         <f aca="false">A31*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B31*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C31*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D31*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E31*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F31*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G31*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H31*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>6.40636092219369</v>
       </c>
       <c r="K31" s="9"/>
       <c r="L31" s="9"/>
@@ -1571,7 +1571,7 @@
       <c r="I32" s="9"/>
       <c r="J32" s="10" t="n">
         <f aca="false">A32*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B32*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C32*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D32*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E32*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F32*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G32*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H32*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>6.99645755068471</v>
       </c>
       <c r="K32" s="10"/>
       <c r="L32" s="10"/>
@@ -1610,7 +1610,7 @@
       <c r="I33" s="9"/>
       <c r="J33" s="9" t="n">
         <f aca="false">A33*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B33*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C33*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D33*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E33*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F33*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G33*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H33*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>7.67350597342476</v>
       </c>
       <c r="K33" s="9"/>
       <c r="L33" s="9"/>
@@ -1649,7 +1649,7 @@
       <c r="I34" s="9"/>
       <c r="J34" s="10" t="n">
         <f aca="false">A34*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B34*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C34*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D34*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E34*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F34*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G34*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H34*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>8.34209230428578</v>
       </c>
       <c r="K34" s="10"/>
       <c r="L34" s="10"/>
@@ -1688,7 +1688,7 @@
       <c r="I35" s="9"/>
       <c r="J35" s="9" t="n">
         <f aca="false">A35*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B35*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C35*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D35*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E35*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F35*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G35*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H35*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>8.70393033882094</v>
       </c>
       <c r="K35" s="9"/>
       <c r="L35" s="9"/>
@@ -1727,7 +1727,7 @@
       <c r="I36" s="9"/>
       <c r="J36" s="10" t="n">
         <f aca="false">A36*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B36*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C36*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D36*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E36*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F36*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G36*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H36*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>8.84074766960155</v>
       </c>
       <c r="K36" s="10"/>
       <c r="L36" s="10"/>
@@ -1766,7 +1766,7 @@
       <c r="I37" s="9"/>
       <c r="J37" s="9" t="n">
         <f aca="false">A37*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B37*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C37*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D37*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E37*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F37*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G37*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H37*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>8.99233059067269</v>
       </c>
       <c r="K37" s="9"/>
       <c r="L37" s="9"/>
@@ -1805,7 +1805,7 @@
       <c r="I38" s="9"/>
       <c r="J38" s="10" t="n">
         <f aca="false">A38*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B38*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C38*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D38*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E38*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F38*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G38*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H38*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>9.21286182550102</v>
       </c>
       <c r="K38" s="10"/>
       <c r="L38" s="10"/>
@@ -1844,7 +1844,7 @@
       <c r="I39" s="9"/>
       <c r="J39" s="9" t="n">
         <f aca="false">A39*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B39*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C39*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D39*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E39*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F39*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G39*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H39*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>9.32826550359735</v>
       </c>
       <c r="K39" s="9"/>
       <c r="L39" s="9"/>
@@ -1883,7 +1883,7 @@
       <c r="I40" s="9"/>
       <c r="J40" s="10" t="n">
         <f aca="false">A40*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B40*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C40*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D40*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E40*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F40*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G40*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H40*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>9.25158983071263</v>
       </c>
       <c r="K40" s="10"/>
       <c r="L40" s="10"/>
@@ -1922,7 +1922,7 @@
       <c r="I41" s="9"/>
       <c r="J41" s="9" t="n">
         <f aca="false">A41*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B41*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C41*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D41*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E41*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F41*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G41*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H41*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>9.22585899109326</v>
       </c>
       <c r="K41" s="9"/>
       <c r="L41" s="9"/>
@@ -1961,7 +1961,7 @@
       <c r="I42" s="9"/>
       <c r="J42" s="10" t="n">
         <f aca="false">A42*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B42*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C42*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D42*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E42*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F42*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G42*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H42*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>9.32002129849643</v>
       </c>
       <c r="K42" s="10"/>
       <c r="L42" s="10"/>
@@ -2000,7 +2000,7 @@
       <c r="I43" s="9"/>
       <c r="J43" s="9" t="n">
         <f aca="false">A43*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B43*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C43*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D43*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E43*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F43*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G43*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H43*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>9.52777325451064</v>
       </c>
       <c r="K43" s="9"/>
       <c r="L43" s="9"/>
@@ -2039,7 +2039,7 @@
       <c r="I44" s="9"/>
       <c r="J44" s="10" t="n">
         <f aca="false">A44*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B44*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C44*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D44*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E44*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F44*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G44*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H44*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>9.71860102676678</v>
       </c>
       <c r="K44" s="10"/>
       <c r="L44" s="10"/>
@@ -2078,7 +2078,7 @@
       <c r="I45" s="9"/>
       <c r="J45" s="9" t="n">
         <f aca="false">A45*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B45*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C45*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D45*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E45*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F45*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G45*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H45*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>9.87450113477301</v>
       </c>
       <c r="K45" s="9"/>
       <c r="L45" s="9"/>
@@ -2117,7 +2117,7 @@
       <c r="I46" s="9"/>
       <c r="J46" s="10" t="n">
         <f aca="false">A46*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B46*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C46*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D46*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E46*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F46*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G46*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H46*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>10.0856632629797</v>
       </c>
       <c r="K46" s="10"/>
       <c r="L46" s="10"/>
@@ -2156,7 +2156,7 @@
       <c r="I47" s="9"/>
       <c r="J47" s="9" t="n">
         <f aca="false">A47*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B47*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C47*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D47*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E47*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F47*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G47*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H47*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>10.5420081689003</v>
       </c>
       <c r="K47" s="9"/>
       <c r="L47" s="9"/>
@@ -2195,7 +2195,7 @@
       <c r="I48" s="9"/>
       <c r="J48" s="10" t="n">
         <f aca="false">A48*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B48*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C48*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D48*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E48*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F48*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G48*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H48*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>11.2636979264942</v>
       </c>
       <c r="K48" s="10"/>
       <c r="L48" s="10"/>
@@ -2234,7 +2234,7 @@
       <c r="I49" s="9"/>
       <c r="J49" s="9" t="n">
         <f aca="false">A49*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B49*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C49*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D49*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E49*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F49*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G49*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H49*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>12.0714324635945</v>
       </c>
       <c r="K49" s="9"/>
       <c r="L49" s="9"/>
@@ -2273,7 +2273,7 @@
       <c r="I50" s="9"/>
       <c r="J50" s="10" t="n">
         <f aca="false">A50*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B50*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C50*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D50*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E50*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F50*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G50*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H50*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>12.9725945753464</v>
       </c>
       <c r="K50" s="10"/>
       <c r="L50" s="10"/>
@@ -2312,7 +2312,7 @@
       <c r="I51" s="9"/>
       <c r="J51" s="9" t="n">
         <f aca="false">A51*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B51*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C51*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D51*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E51*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F51*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G51*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H51*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>13.9767256503629</v>
       </c>
       <c r="K51" s="9"/>
       <c r="L51" s="9"/>
@@ -2351,7 +2351,7 @@
       <c r="I52" s="9"/>
       <c r="J52" s="10" t="n">
         <f aca="false">A52*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B52*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C52*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D52*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E52*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F52*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G52*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H52*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>15.1623153910137</v>
       </c>
       <c r="K52" s="10"/>
       <c r="L52" s="10"/>
@@ -2390,7 +2390,7 @@
       <c r="I53" s="9"/>
       <c r="J53" s="9" t="n">
         <f aca="false">A53*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B53*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C53*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D53*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E53*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F53*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G53*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H53*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>16.4604154835419</v>
       </c>
       <c r="K53" s="9"/>
       <c r="L53" s="9"/>
@@ -2429,7 +2429,7 @@
       <c r="I54" s="9"/>
       <c r="J54" s="10" t="n">
         <f aca="false">A54*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B54*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C54*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D54*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E54*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F54*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G54*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H54*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>17.5451948543959</v>
       </c>
       <c r="K54" s="10"/>
       <c r="L54" s="10"/>
@@ -2468,7 +2468,7 @@
       <c r="I55" s="9"/>
       <c r="J55" s="9" t="n">
         <f aca="false">A55*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B55*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C55*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D55*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E55*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F55*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G55*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H55*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>18.2744396891262</v>
       </c>
       <c r="K55" s="9"/>
       <c r="L55" s="9"/>
@@ -2507,7 +2507,7 @@
       <c r="I56" s="9"/>
       <c r="J56" s="10" t="n">
         <f aca="false">A56*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B56*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C56*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D56*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E56*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F56*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G56*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H56*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>18.7192568949576</v>
       </c>
       <c r="K56" s="10"/>
       <c r="L56" s="10"/>
@@ -2546,7 +2546,7 @@
       <c r="I57" s="9"/>
       <c r="J57" s="9" t="n">
         <f aca="false">A57*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B57*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C57*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D57*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E57*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F57*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G57*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H57*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>19.0738844163386</v>
       </c>
       <c r="K57" s="9"/>
       <c r="L57" s="9"/>
@@ -2585,7 +2585,7 @@
       <c r="I58" s="9"/>
       <c r="J58" s="10" t="n">
         <f aca="false">A58*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B58*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C58*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D58*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E58*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F58*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G58*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H58*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>19.4465154182114</v>
       </c>
       <c r="K58" s="10"/>
       <c r="L58" s="10"/>
@@ -2624,7 +2624,7 @@
       <c r="I59" s="9"/>
       <c r="J59" s="9" t="n">
         <f aca="false">A59*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B59*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C59*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D59*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E59*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F59*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G59*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H59*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>19.7658423270801</v>
       </c>
       <c r="K59" s="9"/>
       <c r="L59" s="9"/>
@@ -2663,7 +2663,7 @@
       <c r="I60" s="9"/>
       <c r="J60" s="10" t="n">
         <f aca="false">A60*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B60*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C60*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D60*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E60*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F60*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G60*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H60*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>19.9175833380022</v>
       </c>
       <c r="K60" s="10"/>
       <c r="L60" s="10"/>
@@ -2702,7 +2702,7 @@
       <c r="I61" s="9"/>
       <c r="J61" s="9" t="n">
         <f aca="false">A61*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B61*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C61*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D61*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E61*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F61*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G61*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H61*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>19.7614967558648</v>
       </c>
       <c r="K61" s="9"/>
       <c r="L61" s="9"/>
@@ -2741,7 +2741,7 @@
       <c r="I62" s="9"/>
       <c r="J62" s="10" t="n">
         <f aca="false">A62*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B62*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C62*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D62*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E62*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F62*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G62*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H62*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>18.9794788662437</v>
       </c>
       <c r="K62" s="10"/>
       <c r="L62" s="10"/>
@@ -2780,7 +2780,7 @@
       <c r="I63" s="9"/>
       <c r="J63" s="9" t="n">
         <f aca="false">A63*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B63*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C63*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D63*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E63*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F63*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G63*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H63*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>17.9798230680134</v>
       </c>
       <c r="K63" s="9"/>
       <c r="L63" s="9"/>
@@ -2819,7 +2819,7 @@
       <c r="I64" s="9"/>
       <c r="J64" s="10" t="n">
         <f aca="false">A64*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B64*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C64*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D64*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E64*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F64*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G64*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H64*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>16.7677393707114</v>
       </c>
       <c r="K64" s="10"/>
       <c r="L64" s="10"/>
@@ -2858,7 +2858,7 @@
       <c r="I65" s="9"/>
       <c r="J65" s="9" t="n">
         <f aca="false">A65*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B65*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C65*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D65*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E65*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F65*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G65*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H65*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>15.6872346103721</v>
       </c>
       <c r="K65" s="9"/>
       <c r="L65" s="9"/>
@@ -2897,7 +2897,7 @@
       <c r="I66" s="9"/>
       <c r="J66" s="10" t="n">
         <f aca="false">A66*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B66*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C66*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D66*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E66*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F66*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G66*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H66*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>14.7465844047435</v>
       </c>
       <c r="K66" s="10"/>
       <c r="L66" s="10"/>
@@ -2936,7 +2936,7 @@
       <c r="I67" s="9"/>
       <c r="J67" s="9" t="n">
         <f aca="false">A67*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B67*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C67*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D67*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E67*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F67*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G67*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H67*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>13.8746676544605</v>
       </c>
       <c r="K67" s="9"/>
       <c r="L67" s="9"/>
@@ -2975,7 +2975,7 @@
       <c r="I68" s="9"/>
       <c r="J68" s="10" t="n">
         <f aca="false">A68*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B68*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C68*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D68*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E68*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F68*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G68*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H68*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>13.0224974534541</v>
       </c>
       <c r="K68" s="10"/>
       <c r="L68" s="10"/>
@@ -3014,7 +3014,7 @@
       <c r="I69" s="9"/>
       <c r="J69" s="9" t="n">
         <f aca="false">A69*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B69*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C69*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D69*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E69*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F69*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G69*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H69*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>12.2566486636024</v>
       </c>
       <c r="K69" s="9"/>
       <c r="L69" s="9"/>
@@ -3053,7 +3053,7 @@
       <c r="I70" s="9"/>
       <c r="J70" s="10" t="n">
         <f aca="false">A70*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B70*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C70*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D70*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E70*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F70*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G70*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H70*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>11.6742782398182</v>
       </c>
       <c r="K70" s="10"/>
       <c r="L70" s="10"/>
@@ -3092,7 +3092,7 @@
       <c r="I71" s="9"/>
       <c r="J71" s="9" t="n">
         <f aca="false">A71*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B71*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C71*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D71*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E71*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F71*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G71*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H71*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>11.4585879165207</v>
       </c>
       <c r="K71" s="9"/>
       <c r="L71" s="9"/>
@@ -3131,7 +3131,7 @@
       <c r="I72" s="9"/>
       <c r="J72" s="10" t="n">
         <f aca="false">A72*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B72*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C72*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D72*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E72*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F72*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G72*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H72*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>11.8205867367418</v>
       </c>
       <c r="K72" s="10"/>
       <c r="L72" s="10"/>
@@ -3170,7 +3170,7 @@
       <c r="I73" s="9"/>
       <c r="J73" s="9" t="n">
         <f aca="false">A73*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B73*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C73*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D73*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E73*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F73*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G73*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H73*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>12.9543737518957</v>
       </c>
       <c r="K73" s="9"/>
       <c r="L73" s="9"/>
@@ -3209,7 +3209,7 @@
       <c r="I74" s="9"/>
       <c r="J74" s="10" t="n">
         <f aca="false">A74*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B74*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C74*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D74*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E74*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F74*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G74*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H74*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>15.2172883401276</v>
       </c>
       <c r="K74" s="10"/>
       <c r="L74" s="10"/>
@@ -3248,7 +3248,7 @@
       <c r="I75" s="9"/>
       <c r="J75" s="9" t="n">
         <f aca="false">A75*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B75*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C75*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D75*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E75*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F75*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G75*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H75*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>18.4250494702845</v>
       </c>
       <c r="K75" s="9"/>
       <c r="L75" s="9"/>
@@ -3287,7 +3287,7 @@
       <c r="I76" s="9"/>
       <c r="J76" s="10" t="n">
         <f aca="false">A76*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B76*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C76*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D76*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E76*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F76*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G76*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H76*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>20.6365561194714</v>
       </c>
       <c r="K76" s="10"/>
       <c r="L76" s="10"/>
@@ -3326,7 +3326,7 @@
       <c r="I77" s="9"/>
       <c r="J77" s="9" t="n">
         <f aca="false">A77*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B77*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C77*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D77*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E77*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F77*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G77*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H77*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>19.8215634881202</v>
       </c>
       <c r="K77" s="9"/>
       <c r="L77" s="9"/>
@@ -3365,7 +3365,7 @@
       <c r="I78" s="9"/>
       <c r="J78" s="10" t="n">
         <f aca="false">A78*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B78*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C78*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D78*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E78*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F78*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G78*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H78*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>15.1755426947961</v>
       </c>
       <c r="K78" s="10"/>
       <c r="L78" s="10"/>
@@ -3404,7 +3404,7 @@
       <c r="I79" s="9"/>
       <c r="J79" s="9" t="n">
         <f aca="false">A79*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B79*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C79*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D79*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E79*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F79*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G79*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H79*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>10.0519651635591</v>
       </c>
       <c r="K79" s="9"/>
       <c r="L79" s="9"/>
@@ -3443,7 +3443,7 @@
       <c r="I80" s="9"/>
       <c r="J80" s="10" t="n">
         <f aca="false">A80*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B80*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C80*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D80*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E80*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F80*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G80*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H80*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>6.62072958241667</v>
       </c>
       <c r="K80" s="10"/>
       <c r="L80" s="10"/>
@@ -3482,7 +3482,7 @@
       <c r="I81" s="9"/>
       <c r="J81" s="9" t="n">
         <f aca="false">A81*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B81*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C81*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D81*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E81*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F81*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G81*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H81*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>4.72568759599449</v>
       </c>
       <c r="K81" s="9"/>
       <c r="L81" s="9"/>
@@ -3521,7 +3521,7 @@
       <c r="I82" s="9"/>
       <c r="J82" s="10" t="n">
         <f aca="false">A82*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B82*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C82*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D82*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E82*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F82*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G82*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H82*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>3.70694517028287</v>
       </c>
       <c r="K82" s="10"/>
       <c r="L82" s="10"/>
@@ -3560,7 +3560,7 @@
       <c r="I83" s="9"/>
       <c r="J83" s="9" t="n">
         <f aca="false">A83*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B83*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C83*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D83*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E83*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F83*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G83*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H83*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>3.07680217994211</v>
       </c>
       <c r="K83" s="9"/>
       <c r="L83" s="9"/>
@@ -3599,7 +3599,7 @@
       <c r="I84" s="9"/>
       <c r="J84" s="10" t="n">
         <f aca="false">A84*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B84*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C84*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D84*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E84*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F84*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G84*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H84*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>2.58569688708636</v>
       </c>
       <c r="K84" s="10"/>
       <c r="L84" s="10"/>
@@ -3638,7 +3638,7 @@
       <c r="I85" s="9"/>
       <c r="J85" s="9" t="n">
         <f aca="false">A85*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B85*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C85*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D85*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E85*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F85*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G85*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H85*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>2.23638988399722</v>
       </c>
       <c r="K85" s="9"/>
       <c r="L85" s="9"/>
@@ -3677,7 +3677,7 @@
       <c r="I86" s="9"/>
       <c r="J86" s="10" t="n">
         <f aca="false">A86*(((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000)*$A$3*(((1-((((100/MAX($K$2:$R$2))*$K$2)*10)*($K$3/100)/1000))*$A$4)+1))/A$5+B86*(((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000)*$B$3*(((1-((((100/MAX($K$2:$R$2))*$L$2)*10)*($K$3/100)/1000))*$B$4)+1))/B$5+C86*(((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000)*$C$3*(((1-((((100/MAX($K$2:$R$2))*$M$2)*10)*($K$3/100)/1000))*$C$4)+1))/C$5+D86*(((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000)*$D$3*(((1-((((100/MAX($K$2:$R$2))*$N$2)*10)*($K$3/100)/1000))*$D$4)+1))/D$5+E86*(((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000)*$E$3*(((1-((((100/MAX($K$2:$R$2))*$O$2)*10)*($K$3/100)/1000))*$E$4)+1))/E$5+F86*(((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000)*$F$3*(((1-((((100/MAX($K$2:$R$2))*$P$2)*10)*($K$3/100)/1000))*$F$4)+1))/F$5+G86*(((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000)*$G$3*(((1-((((100/MAX($K$2:$R$2))*$Q$2)*10)*($K$3/100)/1000))*$G$4)+1))/G$5+H86*(((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000)*$H$3*(((1-((((100/MAX($K$2:$R$2))*$R$2)*10)*($K$3/100)/1000))*$H$4)+1))/H$5</f>
-        <v>0</v>
+        <v>1.8420260213714</v>
       </c>
       <c r="K86" s="10"/>
       <c r="L86" s="10"/>
@@ -3693,7 +3693,7 @@
     <mergeCell ref="A1:R1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.277777777777778"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.277777777777778"/>
   <pageSetup paperSize="1" scale="72" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>

</xml_diff>